<commit_message>
added the momentum calculations
</commit_message>
<xml_diff>
--- a/1_Data/Data_ETF_YIELDS_1.0.xlsx
+++ b/1_Data/Data_ETF_YIELDS_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Corinne Vogel\Documents\UZH\Master 2. Semester\PMP\Code\PMP-Term-Paper\1_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81DF5E2F-BD4E-4932-94D3-3F25D047E137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B988E86-195B-4BD5-AB6C-F7B01AD386E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Needs Mapped" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <definedName name="SpreadsheetBuilder_2" hidden="1">ETF_TR!$A$2:$P$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2606,8 +2605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P282"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="87" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -16722,7 +16721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BN282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
       <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
@@ -71460,8 +71459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677D5B4D-8910-48A5-9AA1-B185E4342A35}">
   <dimension ref="A1:Z282"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Z1048576"/>
+    <sheetView zoomScale="51" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
further changes in code
</commit_message>
<xml_diff>
--- a/1_Data/Data_ETF_YIELDS_1.0.xlsx
+++ b/1_Data/Data_ETF_YIELDS_1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Corinne Vogel\Documents\UZH\Master 2. Semester\PMP\Code\PMP-Term-Paper\1_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE294BED-D958-42AC-BAA7-95BAFE6A12EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6FD7BE-CDE9-47D4-BA49-476E0DBC15C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Needs Mapped" sheetId="1" r:id="rId1"/>
@@ -2605,7 +2605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P282"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="87" workbookViewId="0">
+      <selection activeCell="G281" sqref="G281:I281"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
@@ -16719,9 +16721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BN282"/>
   <sheetViews>
-    <sheetView topLeftCell="A235" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
@@ -71457,7 +71457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{677D5B4D-8910-48A5-9AA1-B185E4342A35}">
   <dimension ref="A1:AA282"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
+    <sheetView zoomScale="62" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>